<commit_message>
fix data for BL11 inv for 13/2/2024
</commit_message>
<xml_diff>
--- a/data/s1/2024/2/13/S1_BL11/13_02_2024-S1_BL11.xlsx
+++ b/data/s1/2024/2/13/S1_BL11/13_02_2024-S1_BL11.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM573"/>
+  <dimension ref="A1:AM615"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -67545,6 +67545,4920 @@
       <c r="AL573" t="inlineStr"/>
       <c r="AM573" t="inlineStr"/>
     </row>
+    <row r="574">
+      <c r="A574" s="1" t="n">
+        <v>45335.62703703704</v>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C574" t="n">
+        <v>560.8</v>
+      </c>
+      <c r="D574" t="n">
+        <v>451.2</v>
+      </c>
+      <c r="E574" t="n">
+        <v>560.3</v>
+      </c>
+      <c r="F574" t="n">
+        <v>558.2</v>
+      </c>
+      <c r="G574" t="n">
+        <v>4</v>
+      </c>
+      <c r="H574" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="I574" t="n">
+        <v>2</v>
+      </c>
+      <c r="J574" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="K574" t="n">
+        <v>233.6</v>
+      </c>
+      <c r="L574" t="n">
+        <v>234.2</v>
+      </c>
+      <c r="M574" t="n">
+        <v>235.2</v>
+      </c>
+      <c r="N574" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="O574" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="P574" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="Q574" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="R574" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="S574" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="T574" t="n">
+        <v>7216</v>
+      </c>
+      <c r="U574" t="n">
+        <v>1</v>
+      </c>
+      <c r="V574" t="n">
+        <v>50.1</v>
+      </c>
+      <c r="W574" t="n">
+        <v>37621</v>
+      </c>
+      <c r="X574" t="n">
+        <v>3725</v>
+      </c>
+      <c r="Y574" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Z574" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="AA574" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AB574" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC574" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD574" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="AE574" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF574" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG574" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="AH574" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI574" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ574" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK574" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL574" t="inlineStr"/>
+      <c r="AM574" t="inlineStr"/>
+    </row>
+    <row r="575">
+      <c r="A575" s="1" t="n">
+        <v>45335.63050925926</v>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C575" t="n">
+        <v>573.9</v>
+      </c>
+      <c r="D575" t="n">
+        <v>447</v>
+      </c>
+      <c r="E575" t="n">
+        <v>559.3</v>
+      </c>
+      <c r="F575" t="n">
+        <v>551.8</v>
+      </c>
+      <c r="G575" t="n">
+        <v>5</v>
+      </c>
+      <c r="H575" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="I575" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="J575" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="K575" t="n">
+        <v>234.2</v>
+      </c>
+      <c r="L575" t="n">
+        <v>234.4</v>
+      </c>
+      <c r="M575" t="n">
+        <v>235.4</v>
+      </c>
+      <c r="N575" t="n">
+        <v>24.4</v>
+      </c>
+      <c r="O575" t="n">
+        <v>24.3</v>
+      </c>
+      <c r="P575" t="n">
+        <v>24.1</v>
+      </c>
+      <c r="Q575" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="R575" t="n">
+        <v>59.96</v>
+      </c>
+      <c r="S575" t="n">
+        <v>59.97</v>
+      </c>
+      <c r="T575" t="n">
+        <v>11002</v>
+      </c>
+      <c r="U575" t="n">
+        <v>1</v>
+      </c>
+      <c r="V575" t="n">
+        <v>50.2</v>
+      </c>
+      <c r="W575" t="n">
+        <v>37622.2</v>
+      </c>
+      <c r="X575" t="n">
+        <v>3725</v>
+      </c>
+      <c r="Y575" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z575" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="AA575" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB575" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AC575" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="AD575" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="AE575" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AF575" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG575" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH575" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI575" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ575" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK575" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL575" t="inlineStr"/>
+      <c r="AM575" t="inlineStr"/>
+    </row>
+    <row r="576">
+      <c r="A576" s="1" t="n">
+        <v>45335.63398148148</v>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C576" t="n">
+        <v>564.2</v>
+      </c>
+      <c r="D576" t="n">
+        <v>443.7</v>
+      </c>
+      <c r="E576" t="n">
+        <v>558.9</v>
+      </c>
+      <c r="F576" t="n">
+        <v>556.5</v>
+      </c>
+      <c r="G576" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="H576" t="n">
+        <v>12.3</v>
+      </c>
+      <c r="I576" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="J576" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K576" t="n">
+        <v>234.8</v>
+      </c>
+      <c r="L576" t="n">
+        <v>235</v>
+      </c>
+      <c r="M576" t="n">
+        <v>236.4</v>
+      </c>
+      <c r="N576" t="n">
+        <v>38.2</v>
+      </c>
+      <c r="O576" t="n">
+        <v>38.3</v>
+      </c>
+      <c r="P576" t="n">
+        <v>37.9</v>
+      </c>
+      <c r="Q576" t="n">
+        <v>59.97</v>
+      </c>
+      <c r="R576" t="n">
+        <v>60</v>
+      </c>
+      <c r="S576" t="n">
+        <v>60.02</v>
+      </c>
+      <c r="T576" t="n">
+        <v>15389</v>
+      </c>
+      <c r="U576" t="n">
+        <v>1</v>
+      </c>
+      <c r="V576" t="n">
+        <v>50.7</v>
+      </c>
+      <c r="W576" t="n">
+        <v>37623.4</v>
+      </c>
+      <c r="X576" t="n">
+        <v>3726</v>
+      </c>
+      <c r="Y576" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Z576" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="AA576" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB576" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="AC576" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="AD576" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="AE576" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="AF576" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG576" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="AH576" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI576" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ576" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK576" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL576" t="inlineStr"/>
+      <c r="AM576" t="inlineStr"/>
+    </row>
+    <row r="577">
+      <c r="A577" s="1" t="n">
+        <v>45335.6374537037</v>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C577" t="n">
+        <v>555.1</v>
+      </c>
+      <c r="D577" t="n">
+        <v>444.9</v>
+      </c>
+      <c r="E577" t="n">
+        <v>556.9</v>
+      </c>
+      <c r="F577" t="n">
+        <v>547.7</v>
+      </c>
+      <c r="G577" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="H577" t="n">
+        <v>12</v>
+      </c>
+      <c r="I577" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="J577" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="K577" t="n">
+        <v>235</v>
+      </c>
+      <c r="L577" t="n">
+        <v>235.2</v>
+      </c>
+      <c r="M577" t="n">
+        <v>235.2</v>
+      </c>
+      <c r="N577" t="n">
+        <v>36.9</v>
+      </c>
+      <c r="O577" t="n">
+        <v>36.9</v>
+      </c>
+      <c r="P577" t="n">
+        <v>36.9</v>
+      </c>
+      <c r="Q577" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="R577" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="S577" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="T577" t="n">
+        <v>14571</v>
+      </c>
+      <c r="U577" t="n">
+        <v>1</v>
+      </c>
+      <c r="V577" t="n">
+        <v>51.2</v>
+      </c>
+      <c r="W577" t="n">
+        <v>37624.6</v>
+      </c>
+      <c r="X577" t="n">
+        <v>3726</v>
+      </c>
+      <c r="Y577" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z577" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="AA577" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AB577" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="AC577" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="AD577" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="AE577" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="AF577" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG577" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="AH577" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI577" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ577" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK577" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL577" t="inlineStr"/>
+      <c r="AM577" t="inlineStr"/>
+    </row>
+    <row r="578">
+      <c r="A578" s="1" t="n">
+        <v>45335.64091435185</v>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C578" t="n">
+        <v>559.2</v>
+      </c>
+      <c r="D578" t="n">
+        <v>441.8</v>
+      </c>
+      <c r="E578" t="n">
+        <v>562.3</v>
+      </c>
+      <c r="F578" t="n">
+        <v>554</v>
+      </c>
+      <c r="G578" t="n">
+        <v>7</v>
+      </c>
+      <c r="H578" t="n">
+        <v>10</v>
+      </c>
+      <c r="I578" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="J578" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K578" t="n">
+        <v>234.4</v>
+      </c>
+      <c r="L578" t="n">
+        <v>234.6</v>
+      </c>
+      <c r="M578" t="n">
+        <v>235.6</v>
+      </c>
+      <c r="N578" t="n">
+        <v>31.2</v>
+      </c>
+      <c r="O578" t="n">
+        <v>30.9</v>
+      </c>
+      <c r="P578" t="n">
+        <v>31.1</v>
+      </c>
+      <c r="Q578" t="n">
+        <v>59.93</v>
+      </c>
+      <c r="R578" t="n">
+        <v>59.93</v>
+      </c>
+      <c r="S578" t="n">
+        <v>59.91</v>
+      </c>
+      <c r="T578" t="n">
+        <v>12449</v>
+      </c>
+      <c r="U578" t="n">
+        <v>1</v>
+      </c>
+      <c r="V578" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="W578" t="n">
+        <v>37625.7</v>
+      </c>
+      <c r="X578" t="n">
+        <v>3726</v>
+      </c>
+      <c r="Y578" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z578" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="AA578" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="AB578" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="AC578" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AD578" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="AE578" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="AF578" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG578" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH578" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI578" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ578" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK578" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL578" t="inlineStr"/>
+      <c r="AM578" t="inlineStr"/>
+    </row>
+    <row r="579">
+      <c r="A579" s="1" t="n">
+        <v>45335.64440972222</v>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C579" t="n">
+        <v>562</v>
+      </c>
+      <c r="D579" t="n">
+        <v>446.3</v>
+      </c>
+      <c r="E579" t="n">
+        <v>556.3</v>
+      </c>
+      <c r="F579" t="n">
+        <v>556.9</v>
+      </c>
+      <c r="G579" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="H579" t="n">
+        <v>9</v>
+      </c>
+      <c r="I579" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J579" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="K579" t="n">
+        <v>234.4</v>
+      </c>
+      <c r="L579" t="n">
+        <v>234</v>
+      </c>
+      <c r="M579" t="n">
+        <v>236.2</v>
+      </c>
+      <c r="N579" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="O579" t="n">
+        <v>28.7</v>
+      </c>
+      <c r="P579" t="n">
+        <v>28.4</v>
+      </c>
+      <c r="Q579" t="n">
+        <v>59.97</v>
+      </c>
+      <c r="R579" t="n">
+        <v>60</v>
+      </c>
+      <c r="S579" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="T579" t="n">
+        <v>11223</v>
+      </c>
+      <c r="U579" t="n">
+        <v>1</v>
+      </c>
+      <c r="V579" t="n">
+        <v>51.7</v>
+      </c>
+      <c r="W579" t="n">
+        <v>37626.7</v>
+      </c>
+      <c r="X579" t="n">
+        <v>3726</v>
+      </c>
+      <c r="Y579" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z579" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="AA579" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="AB579" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="AC579" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="AD579" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="AE579" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="AF579" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG579" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="AH579" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI579" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ579" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK579" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL579" t="inlineStr"/>
+      <c r="AM579" t="inlineStr"/>
+    </row>
+    <row r="580">
+      <c r="A580" s="1" t="n">
+        <v>45335.64787037037</v>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C580" t="n">
+        <v>558.5</v>
+      </c>
+      <c r="D580" t="n">
+        <v>445</v>
+      </c>
+      <c r="E580" t="n">
+        <v>556.6</v>
+      </c>
+      <c r="F580" t="n">
+        <v>553.3</v>
+      </c>
+      <c r="G580" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="H580" t="n">
+        <v>9</v>
+      </c>
+      <c r="I580" t="n">
+        <v>3</v>
+      </c>
+      <c r="J580" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="K580" t="n">
+        <v>234.6</v>
+      </c>
+      <c r="L580" t="n">
+        <v>234.2</v>
+      </c>
+      <c r="M580" t="n">
+        <v>235.4</v>
+      </c>
+      <c r="N580" t="n">
+        <v>28</v>
+      </c>
+      <c r="O580" t="n">
+        <v>27.8</v>
+      </c>
+      <c r="P580" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="Q580" t="n">
+        <v>60.03</v>
+      </c>
+      <c r="R580" t="n">
+        <v>60.07</v>
+      </c>
+      <c r="S580" t="n">
+        <v>60.05</v>
+      </c>
+      <c r="T580" t="n">
+        <v>11123</v>
+      </c>
+      <c r="U580" t="n">
+        <v>1</v>
+      </c>
+      <c r="V580" t="n">
+        <v>51.6</v>
+      </c>
+      <c r="W580" t="n">
+        <v>37627.6</v>
+      </c>
+      <c r="X580" t="n">
+        <v>3726</v>
+      </c>
+      <c r="Y580" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Z580" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AA580" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AB580" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC580" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="AD580" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="AE580" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="AF580" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG580" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AH580" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI580" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ580" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK580" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL580" t="inlineStr"/>
+      <c r="AM580" t="inlineStr"/>
+    </row>
+    <row r="581">
+      <c r="A581" s="1" t="n">
+        <v>45335.6513425926</v>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C581" t="n">
+        <v>569.6</v>
+      </c>
+      <c r="D581" t="n">
+        <v>454.1</v>
+      </c>
+      <c r="E581" t="n">
+        <v>565.3</v>
+      </c>
+      <c r="F581" t="n">
+        <v>566.1</v>
+      </c>
+      <c r="G581" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="H581" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="I581" t="n">
+        <v>3</v>
+      </c>
+      <c r="J581" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="K581" t="n">
+        <v>234.6</v>
+      </c>
+      <c r="L581" t="n">
+        <v>234.8</v>
+      </c>
+      <c r="M581" t="n">
+        <v>236</v>
+      </c>
+      <c r="N581" t="n">
+        <v>28.6</v>
+      </c>
+      <c r="O581" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="P581" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="Q581" t="n">
+        <v>60.07</v>
+      </c>
+      <c r="R581" t="n">
+        <v>60.04</v>
+      </c>
+      <c r="S581" t="n">
+        <v>60.05</v>
+      </c>
+      <c r="T581" t="n">
+        <v>11386</v>
+      </c>
+      <c r="U581" t="n">
+        <v>1</v>
+      </c>
+      <c r="V581" t="n">
+        <v>51.3</v>
+      </c>
+      <c r="W581" t="n">
+        <v>37628.4</v>
+      </c>
+      <c r="X581" t="n">
+        <v>3726</v>
+      </c>
+      <c r="Y581" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z581" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="AA581" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AB581" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC581" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="AD581" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="AE581" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="AF581" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG581" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AH581" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI581" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ581" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK581" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL581" t="inlineStr"/>
+      <c r="AM581" t="inlineStr"/>
+    </row>
+    <row r="582">
+      <c r="A582" s="1" t="n">
+        <v>45335.65481481481</v>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C582" t="n">
+        <v>570.5</v>
+      </c>
+      <c r="D582" t="n">
+        <v>449.1</v>
+      </c>
+      <c r="E582" t="n">
+        <v>566</v>
+      </c>
+      <c r="F582" t="n">
+        <v>554.9</v>
+      </c>
+      <c r="G582" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="H582" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="I582" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="J582" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="K582" t="n">
+        <v>235.2</v>
+      </c>
+      <c r="L582" t="n">
+        <v>234.6</v>
+      </c>
+      <c r="M582" t="n">
+        <v>236.2</v>
+      </c>
+      <c r="N582" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="O582" t="n">
+        <v>32.4</v>
+      </c>
+      <c r="P582" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="Q582" t="n">
+        <v>60.01</v>
+      </c>
+      <c r="R582" t="n">
+        <v>60.03</v>
+      </c>
+      <c r="S582" t="n">
+        <v>60.01</v>
+      </c>
+      <c r="T582" t="n">
+        <v>12888</v>
+      </c>
+      <c r="U582" t="n">
+        <v>1</v>
+      </c>
+      <c r="V582" t="n">
+        <v>51.4</v>
+      </c>
+      <c r="W582" t="n">
+        <v>37629.5</v>
+      </c>
+      <c r="X582" t="n">
+        <v>3726</v>
+      </c>
+      <c r="Y582" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z582" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA582" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="AB582" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AC582" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="AD582" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="AE582" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="AF582" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG582" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="AH582" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI582" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ582" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK582" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL582" t="inlineStr"/>
+      <c r="AM582" t="inlineStr"/>
+    </row>
+    <row r="583">
+      <c r="A583" s="1" t="n">
+        <v>45335.65828703704</v>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C583" t="n">
+        <v>571.5</v>
+      </c>
+      <c r="D583" t="n">
+        <v>456</v>
+      </c>
+      <c r="E583" t="n">
+        <v>569.4</v>
+      </c>
+      <c r="F583" t="n">
+        <v>565.2</v>
+      </c>
+      <c r="G583" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="H583" t="n">
+        <v>10</v>
+      </c>
+      <c r="I583" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="J583" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K583" t="n">
+        <v>234.6</v>
+      </c>
+      <c r="L583" t="n">
+        <v>235</v>
+      </c>
+      <c r="M583" t="n">
+        <v>236</v>
+      </c>
+      <c r="N583" t="n">
+        <v>31.3</v>
+      </c>
+      <c r="O583" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="P583" t="n">
+        <v>31.2</v>
+      </c>
+      <c r="Q583" t="n">
+        <v>59.97</v>
+      </c>
+      <c r="R583" t="n">
+        <v>59.95</v>
+      </c>
+      <c r="S583" t="n">
+        <v>59.96</v>
+      </c>
+      <c r="T583" t="n">
+        <v>12308</v>
+      </c>
+      <c r="U583" t="n">
+        <v>1</v>
+      </c>
+      <c r="V583" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="W583" t="n">
+        <v>37630.5</v>
+      </c>
+      <c r="X583" t="n">
+        <v>3726</v>
+      </c>
+      <c r="Y583" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Z583" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA583" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="AB583" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="AC583" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="AD583" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="AE583" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="AF583" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG583" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="AH583" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI583" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ583" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK583" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL583" t="inlineStr"/>
+      <c r="AM583" t="inlineStr"/>
+    </row>
+    <row r="584">
+      <c r="A584" s="1" t="n">
+        <v>45335.66175925926</v>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C584" t="n">
+        <v>568.6</v>
+      </c>
+      <c r="D584" t="n">
+        <v>453.1</v>
+      </c>
+      <c r="E584" t="n">
+        <v>565.9</v>
+      </c>
+      <c r="F584" t="n">
+        <v>556.6</v>
+      </c>
+      <c r="G584" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="H584" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="I584" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="J584" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="K584" t="n">
+        <v>234</v>
+      </c>
+      <c r="L584" t="n">
+        <v>234.2</v>
+      </c>
+      <c r="M584" t="n">
+        <v>235.6</v>
+      </c>
+      <c r="N584" t="n">
+        <v>25.1</v>
+      </c>
+      <c r="O584" t="n">
+        <v>25.2</v>
+      </c>
+      <c r="P584" t="n">
+        <v>25.1</v>
+      </c>
+      <c r="Q584" t="n">
+        <v>59.94</v>
+      </c>
+      <c r="R584" t="n">
+        <v>59.91</v>
+      </c>
+      <c r="S584" t="n">
+        <v>59.92</v>
+      </c>
+      <c r="T584" t="n">
+        <v>9688</v>
+      </c>
+      <c r="U584" t="n">
+        <v>1</v>
+      </c>
+      <c r="V584" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="W584" t="n">
+        <v>37631.4</v>
+      </c>
+      <c r="X584" t="n">
+        <v>3726</v>
+      </c>
+      <c r="Y584" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z584" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="AA584" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="AB584" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="AC584" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AD584" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="AE584" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="AF584" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG584" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="AH584" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI584" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ584" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK584" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL584" t="inlineStr"/>
+      <c r="AM584" t="inlineStr"/>
+    </row>
+    <row r="585">
+      <c r="A585" s="1" t="n">
+        <v>45335.66523148148</v>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C585" t="n">
+        <v>571.6</v>
+      </c>
+      <c r="D585" t="n">
+        <v>457.1</v>
+      </c>
+      <c r="E585" t="n">
+        <v>566.8</v>
+      </c>
+      <c r="F585" t="n">
+        <v>561.5</v>
+      </c>
+      <c r="G585" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="H585" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="I585" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J585" t="n">
+        <v>3</v>
+      </c>
+      <c r="K585" t="n">
+        <v>234</v>
+      </c>
+      <c r="L585" t="n">
+        <v>234</v>
+      </c>
+      <c r="M585" t="n">
+        <v>235.4</v>
+      </c>
+      <c r="N585" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="O585" t="n">
+        <v>26.4</v>
+      </c>
+      <c r="P585" t="n">
+        <v>26.1</v>
+      </c>
+      <c r="Q585" t="n">
+        <v>59.97</v>
+      </c>
+      <c r="R585" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="S585" t="n">
+        <v>59.96</v>
+      </c>
+      <c r="T585" t="n">
+        <v>10308</v>
+      </c>
+      <c r="U585" t="n">
+        <v>1</v>
+      </c>
+      <c r="V585" t="n">
+        <v>51.1</v>
+      </c>
+      <c r="W585" t="n">
+        <v>37632.2</v>
+      </c>
+      <c r="X585" t="n">
+        <v>3726</v>
+      </c>
+      <c r="Y585" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z585" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="AA585" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="AB585" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="AC585" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD585" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="AE585" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF585" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG585" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="AH585" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI585" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ585" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK585" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL585" t="inlineStr"/>
+      <c r="AM585" t="inlineStr"/>
+    </row>
+    <row r="586">
+      <c r="A586" s="1" t="n">
+        <v>45335.66871527778</v>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C586" t="n">
+        <v>570.9</v>
+      </c>
+      <c r="D586" t="n">
+        <v>456.4</v>
+      </c>
+      <c r="E586" t="n">
+        <v>573.8</v>
+      </c>
+      <c r="F586" t="n">
+        <v>561.5</v>
+      </c>
+      <c r="G586" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="H586" t="n">
+        <v>7</v>
+      </c>
+      <c r="I586" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J586" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="K586" t="n">
+        <v>234.2</v>
+      </c>
+      <c r="L586" t="n">
+        <v>234.6</v>
+      </c>
+      <c r="M586" t="n">
+        <v>235.2</v>
+      </c>
+      <c r="N586" t="n">
+        <v>22.2</v>
+      </c>
+      <c r="O586" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="P586" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q586" t="n">
+        <v>60.05</v>
+      </c>
+      <c r="R586" t="n">
+        <v>60.05</v>
+      </c>
+      <c r="S586" t="n">
+        <v>60.04</v>
+      </c>
+      <c r="T586" t="n">
+        <v>8731</v>
+      </c>
+      <c r="U586" t="n">
+        <v>1</v>
+      </c>
+      <c r="V586" t="n">
+        <v>51</v>
+      </c>
+      <c r="W586" t="n">
+        <v>37633</v>
+      </c>
+      <c r="X586" t="n">
+        <v>3726</v>
+      </c>
+      <c r="Y586" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z586" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AA586" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="AB586" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="AC586" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AD586" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="AE586" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AF586" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG586" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="AH586" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI586" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ586" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK586" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL586" t="inlineStr"/>
+      <c r="AM586" t="inlineStr"/>
+    </row>
+    <row r="587">
+      <c r="A587" s="1" t="n">
+        <v>45335.6721875</v>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C587" t="n">
+        <v>573.4</v>
+      </c>
+      <c r="D587" t="n">
+        <v>463</v>
+      </c>
+      <c r="E587" t="n">
+        <v>578.9</v>
+      </c>
+      <c r="F587" t="n">
+        <v>570.5</v>
+      </c>
+      <c r="G587" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="H587" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="I587" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="J587" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="K587" t="n">
+        <v>234</v>
+      </c>
+      <c r="L587" t="n">
+        <v>233.8</v>
+      </c>
+      <c r="M587" t="n">
+        <v>235.4</v>
+      </c>
+      <c r="N587" t="n">
+        <v>24.6</v>
+      </c>
+      <c r="O587" t="n">
+        <v>24.7</v>
+      </c>
+      <c r="P587" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="Q587" t="n">
+        <v>59.96</v>
+      </c>
+      <c r="R587" t="n">
+        <v>59.93</v>
+      </c>
+      <c r="S587" t="n">
+        <v>59.95</v>
+      </c>
+      <c r="T587" t="n">
+        <v>9678</v>
+      </c>
+      <c r="U587" t="n">
+        <v>1</v>
+      </c>
+      <c r="V587" t="n">
+        <v>50.6</v>
+      </c>
+      <c r="W587" t="n">
+        <v>37633.7</v>
+      </c>
+      <c r="X587" t="n">
+        <v>3726</v>
+      </c>
+      <c r="Y587" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Z587" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA587" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="AB587" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="AC587" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AD587" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="AE587" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AF587" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG587" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH587" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI587" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ587" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK587" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL587" t="inlineStr"/>
+      <c r="AM587" t="inlineStr"/>
+    </row>
+    <row r="588">
+      <c r="A588" s="1" t="n">
+        <v>45335.67565972222</v>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C588" t="n">
+        <v>571.6</v>
+      </c>
+      <c r="D588" t="n">
+        <v>458.1</v>
+      </c>
+      <c r="E588" t="n">
+        <v>572.5</v>
+      </c>
+      <c r="F588" t="n">
+        <v>565.3</v>
+      </c>
+      <c r="G588" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="H588" t="n">
+        <v>6</v>
+      </c>
+      <c r="I588" t="n">
+        <v>2</v>
+      </c>
+      <c r="J588" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="K588" t="n">
+        <v>233.4</v>
+      </c>
+      <c r="L588" t="n">
+        <v>233.4</v>
+      </c>
+      <c r="M588" t="n">
+        <v>235</v>
+      </c>
+      <c r="N588" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="O588" t="n">
+        <v>19.3</v>
+      </c>
+      <c r="P588" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="Q588" t="n">
+        <v>59.93</v>
+      </c>
+      <c r="R588" t="n">
+        <v>59.92</v>
+      </c>
+      <c r="S588" t="n">
+        <v>59.93</v>
+      </c>
+      <c r="T588" t="n">
+        <v>7722</v>
+      </c>
+      <c r="U588" t="n">
+        <v>1</v>
+      </c>
+      <c r="V588" t="n">
+        <v>50.7</v>
+      </c>
+      <c r="W588" t="n">
+        <v>37634.5</v>
+      </c>
+      <c r="X588" t="n">
+        <v>3727</v>
+      </c>
+      <c r="Y588" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z588" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="AA588" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="AB588" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="AC588" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="AD588" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="AE588" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="AF588" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG588" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="AH588" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI588" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ588" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK588" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL588" t="inlineStr"/>
+      <c r="AM588" t="inlineStr"/>
+    </row>
+    <row r="589">
+      <c r="A589" s="1" t="n">
+        <v>45335.67913194445</v>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C589" t="n">
+        <v>572.2</v>
+      </c>
+      <c r="D589" t="n">
+        <v>461.1</v>
+      </c>
+      <c r="E589" t="n">
+        <v>570.5</v>
+      </c>
+      <c r="F589" t="n">
+        <v>573.2</v>
+      </c>
+      <c r="G589" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="H589" t="n">
+        <v>6</v>
+      </c>
+      <c r="I589" t="n">
+        <v>2</v>
+      </c>
+      <c r="J589" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="K589" t="n">
+        <v>233.4</v>
+      </c>
+      <c r="L589" t="n">
+        <v>233.2</v>
+      </c>
+      <c r="M589" t="n">
+        <v>234.6</v>
+      </c>
+      <c r="N589" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="O589" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="P589" t="n">
+        <v>19.3</v>
+      </c>
+      <c r="Q589" t="n">
+        <v>59.91</v>
+      </c>
+      <c r="R589" t="n">
+        <v>59.94</v>
+      </c>
+      <c r="S589" t="n">
+        <v>59.93</v>
+      </c>
+      <c r="T589" t="n">
+        <v>7506</v>
+      </c>
+      <c r="U589" t="n">
+        <v>1</v>
+      </c>
+      <c r="V589" t="n">
+        <v>50.4</v>
+      </c>
+      <c r="W589" t="n">
+        <v>37635.1</v>
+      </c>
+      <c r="X589" t="n">
+        <v>3727</v>
+      </c>
+      <c r="Y589" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z589" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="AA589" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="AB589" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="AC589" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD589" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="AE589" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF589" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG589" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="AH589" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI589" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ589" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK589" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL589" t="inlineStr"/>
+      <c r="AM589" t="inlineStr"/>
+    </row>
+    <row r="590">
+      <c r="A590" s="1" t="n">
+        <v>45335.6825925926</v>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C590" t="n">
+        <v>580.3</v>
+      </c>
+      <c r="D590" t="n">
+        <v>455</v>
+      </c>
+      <c r="E590" t="n">
+        <v>579.1</v>
+      </c>
+      <c r="F590" t="n">
+        <v>580</v>
+      </c>
+      <c r="G590" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="H590" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="I590" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J590" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="K590" t="n">
+        <v>233.6</v>
+      </c>
+      <c r="L590" t="n">
+        <v>233.4</v>
+      </c>
+      <c r="M590" t="n">
+        <v>235.2</v>
+      </c>
+      <c r="N590" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="O590" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="P590" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="Q590" t="n">
+        <v>60.05</v>
+      </c>
+      <c r="R590" t="n">
+        <v>60.02</v>
+      </c>
+      <c r="S590" t="n">
+        <v>60.05</v>
+      </c>
+      <c r="T590" t="n">
+        <v>6499</v>
+      </c>
+      <c r="U590" t="n">
+        <v>1</v>
+      </c>
+      <c r="V590" t="n">
+        <v>50</v>
+      </c>
+      <c r="W590" t="n">
+        <v>37635.6</v>
+      </c>
+      <c r="X590" t="n">
+        <v>3727</v>
+      </c>
+      <c r="Y590" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z590" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA590" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AB590" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="AC590" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="AD590" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AE590" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="AF590" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG590" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH590" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI590" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ590" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK590" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL590" t="inlineStr"/>
+      <c r="AM590" t="inlineStr"/>
+    </row>
+    <row r="591">
+      <c r="A591" s="1" t="n">
+        <v>45335.68606481481</v>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C591" t="n">
+        <v>578.5</v>
+      </c>
+      <c r="D591" t="n">
+        <v>456</v>
+      </c>
+      <c r="E591" t="n">
+        <v>570</v>
+      </c>
+      <c r="F591" t="n">
+        <v>555.7</v>
+      </c>
+      <c r="G591" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="H591" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="I591" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J591" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K591" t="n">
+        <v>233</v>
+      </c>
+      <c r="L591" t="n">
+        <v>233.2</v>
+      </c>
+      <c r="M591" t="n">
+        <v>234.2</v>
+      </c>
+      <c r="N591" t="n">
+        <v>12.9</v>
+      </c>
+      <c r="O591" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="P591" t="n">
+        <v>13.1</v>
+      </c>
+      <c r="Q591" t="n">
+        <v>60.02</v>
+      </c>
+      <c r="R591" t="n">
+        <v>60.03</v>
+      </c>
+      <c r="S591" t="n">
+        <v>60.03</v>
+      </c>
+      <c r="T591" t="n">
+        <v>5089</v>
+      </c>
+      <c r="U591" t="n">
+        <v>1</v>
+      </c>
+      <c r="V591" t="n">
+        <v>49.2</v>
+      </c>
+      <c r="W591" t="n">
+        <v>37636</v>
+      </c>
+      <c r="X591" t="n">
+        <v>3727</v>
+      </c>
+      <c r="Y591" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z591" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="AA591" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB591" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AC591" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AD591" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="AE591" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="AF591" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG591" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="AH591" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI591" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ591" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK591" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL591" t="inlineStr"/>
+      <c r="AM591" t="inlineStr"/>
+    </row>
+    <row r="592">
+      <c r="A592" s="1" t="n">
+        <v>45335.68953703704</v>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C592" t="n">
+        <v>571.5</v>
+      </c>
+      <c r="D592" t="n">
+        <v>460</v>
+      </c>
+      <c r="E592" t="n">
+        <v>567.7</v>
+      </c>
+      <c r="F592" t="n">
+        <v>561.3</v>
+      </c>
+      <c r="G592" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H592" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="I592" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="J592" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="K592" t="n">
+        <v>232.8</v>
+      </c>
+      <c r="L592" t="n">
+        <v>233</v>
+      </c>
+      <c r="M592" t="n">
+        <v>234.4</v>
+      </c>
+      <c r="N592" t="n">
+        <v>12.4</v>
+      </c>
+      <c r="O592" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="P592" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="Q592" t="n">
+        <v>60.01</v>
+      </c>
+      <c r="R592" t="n">
+        <v>60.02</v>
+      </c>
+      <c r="S592" t="n">
+        <v>60.02</v>
+      </c>
+      <c r="T592" t="n">
+        <v>4765</v>
+      </c>
+      <c r="U592" t="n">
+        <v>1</v>
+      </c>
+      <c r="V592" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="W592" t="n">
+        <v>37636.5</v>
+      </c>
+      <c r="X592" t="n">
+        <v>3727</v>
+      </c>
+      <c r="Y592" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z592" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="AA592" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AB592" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="AC592" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="AD592" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE592" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AF592" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG592" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="AH592" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI592" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ592" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK592" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL592" t="inlineStr"/>
+      <c r="AM592" t="inlineStr"/>
+    </row>
+    <row r="593">
+      <c r="A593" s="1" t="n">
+        <v>45335.69302083334</v>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C593" t="n">
+        <v>573.9</v>
+      </c>
+      <c r="D593" t="n">
+        <v>460.2</v>
+      </c>
+      <c r="E593" t="n">
+        <v>577.5</v>
+      </c>
+      <c r="F593" t="n">
+        <v>559.3</v>
+      </c>
+      <c r="G593" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="H593" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I593" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J593" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="K593" t="n">
+        <v>232.8</v>
+      </c>
+      <c r="L593" t="n">
+        <v>233</v>
+      </c>
+      <c r="M593" t="n">
+        <v>234.6</v>
+      </c>
+      <c r="N593" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="O593" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="P593" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="Q593" t="n">
+        <v>60.04</v>
+      </c>
+      <c r="R593" t="n">
+        <v>60.03</v>
+      </c>
+      <c r="S593" t="n">
+        <v>60.03</v>
+      </c>
+      <c r="T593" t="n">
+        <v>4498</v>
+      </c>
+      <c r="U593" t="n">
+        <v>1</v>
+      </c>
+      <c r="V593" t="n">
+        <v>47.8</v>
+      </c>
+      <c r="W593" t="n">
+        <v>37636.8</v>
+      </c>
+      <c r="X593" t="n">
+        <v>3727</v>
+      </c>
+      <c r="Y593" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z593" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AA593" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AB593" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AC593" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AD593" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AE593" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AF593" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG593" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AH593" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI593" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ593" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK593" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL593" t="inlineStr"/>
+      <c r="AM593" t="inlineStr"/>
+    </row>
+    <row r="594">
+      <c r="A594" s="1" t="n">
+        <v>45335.69649305556</v>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C594" t="n">
+        <v>573.6</v>
+      </c>
+      <c r="D594" t="n">
+        <v>450.1</v>
+      </c>
+      <c r="E594" t="n">
+        <v>577.6</v>
+      </c>
+      <c r="F594" t="n">
+        <v>553.4</v>
+      </c>
+      <c r="G594" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H594" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="I594" t="n">
+        <v>1</v>
+      </c>
+      <c r="J594" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="K594" t="n">
+        <v>232.8</v>
+      </c>
+      <c r="L594" t="n">
+        <v>232.8</v>
+      </c>
+      <c r="M594" t="n">
+        <v>234.8</v>
+      </c>
+      <c r="N594" t="n">
+        <v>10.6</v>
+      </c>
+      <c r="O594" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="P594" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="Q594" t="n">
+        <v>60.02</v>
+      </c>
+      <c r="R594" t="n">
+        <v>60.04</v>
+      </c>
+      <c r="S594" t="n">
+        <v>60.02</v>
+      </c>
+      <c r="T594" t="n">
+        <v>4175</v>
+      </c>
+      <c r="U594" t="n">
+        <v>1</v>
+      </c>
+      <c r="V594" t="n">
+        <v>47.1</v>
+      </c>
+      <c r="W594" t="n">
+        <v>37637.2</v>
+      </c>
+      <c r="X594" t="n">
+        <v>3727</v>
+      </c>
+      <c r="Y594" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z594" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AA594" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AB594" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="AC594" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AD594" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AE594" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="AF594" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG594" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="AH594" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI594" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ594" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK594" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL594" t="inlineStr"/>
+      <c r="AM594" t="inlineStr"/>
+    </row>
+    <row r="595">
+      <c r="A595" s="1" t="n">
+        <v>45335.69996527778</v>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C595" t="n">
+        <v>572.7</v>
+      </c>
+      <c r="D595" t="n">
+        <v>454.9</v>
+      </c>
+      <c r="E595" t="n">
+        <v>572.7</v>
+      </c>
+      <c r="F595" t="n">
+        <v>552.5</v>
+      </c>
+      <c r="G595" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="H595" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="I595" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J595" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="K595" t="n">
+        <v>232.8</v>
+      </c>
+      <c r="L595" t="n">
+        <v>233</v>
+      </c>
+      <c r="M595" t="n">
+        <v>234.2</v>
+      </c>
+      <c r="N595" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="O595" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="P595" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="Q595" t="n">
+        <v>59.94</v>
+      </c>
+      <c r="R595" t="n">
+        <v>59.92</v>
+      </c>
+      <c r="S595" t="n">
+        <v>59.95</v>
+      </c>
+      <c r="T595" t="n">
+        <v>4088</v>
+      </c>
+      <c r="U595" t="n">
+        <v>1</v>
+      </c>
+      <c r="V595" t="n">
+        <v>46.4</v>
+      </c>
+      <c r="W595" t="n">
+        <v>37637.6</v>
+      </c>
+      <c r="X595" t="n">
+        <v>3727</v>
+      </c>
+      <c r="Y595" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z595" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AA595" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AB595" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC595" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="AD595" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AE595" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="AF595" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG595" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="AH595" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI595" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ595" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK595" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL595" t="inlineStr"/>
+      <c r="AM595" t="inlineStr"/>
+    </row>
+    <row r="596">
+      <c r="A596" s="1" t="n">
+        <v>45335.7034375</v>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C596" t="n">
+        <v>556.6</v>
+      </c>
+      <c r="D596" t="n">
+        <v>452.5</v>
+      </c>
+      <c r="E596" t="n">
+        <v>574.8</v>
+      </c>
+      <c r="F596" t="n">
+        <v>531.6</v>
+      </c>
+      <c r="G596" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H596" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="I596" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="J596" t="n">
+        <v>1</v>
+      </c>
+      <c r="K596" t="n">
+        <v>232.8</v>
+      </c>
+      <c r="L596" t="n">
+        <v>232.6</v>
+      </c>
+      <c r="M596" t="n">
+        <v>234.2</v>
+      </c>
+      <c r="N596" t="n">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="O596" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="P596" t="n">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="Q596" t="n">
+        <v>59.94</v>
+      </c>
+      <c r="R596" t="n">
+        <v>59.94</v>
+      </c>
+      <c r="S596" t="n">
+        <v>59.93</v>
+      </c>
+      <c r="T596" t="n">
+        <v>3489</v>
+      </c>
+      <c r="U596" t="n">
+        <v>1</v>
+      </c>
+      <c r="V596" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="W596" t="n">
+        <v>37637.9</v>
+      </c>
+      <c r="X596" t="n">
+        <v>3727</v>
+      </c>
+      <c r="Y596" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z596" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="AA596" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AB596" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AC596" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD596" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AE596" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF596" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG596" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="AH596" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI596" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ596" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK596" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL596" t="inlineStr"/>
+      <c r="AM596" t="inlineStr"/>
+    </row>
+    <row r="597">
+      <c r="A597" s="1" t="n">
+        <v>45335.70690972222</v>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C597" t="n">
+        <v>562.5</v>
+      </c>
+      <c r="D597" t="n">
+        <v>449</v>
+      </c>
+      <c r="E597" t="n">
+        <v>552.7</v>
+      </c>
+      <c r="F597" t="n">
+        <v>496.5</v>
+      </c>
+      <c r="G597" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H597" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="I597" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J597" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K597" t="n">
+        <v>232.8</v>
+      </c>
+      <c r="L597" t="n">
+        <v>232.8</v>
+      </c>
+      <c r="M597" t="n">
+        <v>234.2</v>
+      </c>
+      <c r="N597" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="O597" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="P597" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="Q597" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="R597" t="n">
+        <v>60.01</v>
+      </c>
+      <c r="S597" t="n">
+        <v>60</v>
+      </c>
+      <c r="T597" t="n">
+        <v>2865</v>
+      </c>
+      <c r="U597" t="n">
+        <v>1</v>
+      </c>
+      <c r="V597" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="W597" t="n">
+        <v>37638.1</v>
+      </c>
+      <c r="X597" t="n">
+        <v>3727</v>
+      </c>
+      <c r="Y597" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z597" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AA597" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AB597" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AC597" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AD597" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AE597" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AF597" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG597" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH597" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI597" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ597" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK597" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL597" t="inlineStr"/>
+      <c r="AM597" t="inlineStr"/>
+    </row>
+    <row r="598">
+      <c r="A598" s="1" t="n">
+        <v>45335.71038194445</v>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C598" t="n">
+        <v>552.5</v>
+      </c>
+      <c r="D598" t="n">
+        <v>446.2</v>
+      </c>
+      <c r="E598" t="n">
+        <v>570.7</v>
+      </c>
+      <c r="F598" t="n">
+        <v>495.4</v>
+      </c>
+      <c r="G598" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H598" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="I598" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J598" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K598" t="n">
+        <v>232.2</v>
+      </c>
+      <c r="L598" t="n">
+        <v>232.8</v>
+      </c>
+      <c r="M598" t="n">
+        <v>234.2</v>
+      </c>
+      <c r="N598" t="n">
+        <v>7</v>
+      </c>
+      <c r="O598" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="P598" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="Q598" t="n">
+        <v>60.01</v>
+      </c>
+      <c r="R598" t="n">
+        <v>60.02</v>
+      </c>
+      <c r="S598" t="n">
+        <v>60.01</v>
+      </c>
+      <c r="T598" t="n">
+        <v>2756</v>
+      </c>
+      <c r="U598" t="n">
+        <v>1</v>
+      </c>
+      <c r="V598" t="n">
+        <v>48.1</v>
+      </c>
+      <c r="W598" t="n">
+        <v>37638.4</v>
+      </c>
+      <c r="X598" t="n">
+        <v>3727</v>
+      </c>
+      <c r="Y598" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z598" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AA598" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AB598" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AC598" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AD598" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AE598" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AF598" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG598" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AH598" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI598" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ598" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK598" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL598" t="inlineStr"/>
+      <c r="AM598" t="inlineStr"/>
+    </row>
+    <row r="599">
+      <c r="A599" s="1" t="n">
+        <v>45335.71385416666</v>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C599" t="n">
+        <v>548.5</v>
+      </c>
+      <c r="D599" t="n">
+        <v>448.9</v>
+      </c>
+      <c r="E599" t="n">
+        <v>548.4</v>
+      </c>
+      <c r="F599" t="n">
+        <v>496.1</v>
+      </c>
+      <c r="G599" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H599" t="n">
+        <v>2</v>
+      </c>
+      <c r="I599" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J599" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K599" t="n">
+        <v>233</v>
+      </c>
+      <c r="L599" t="n">
+        <v>232.8</v>
+      </c>
+      <c r="M599" t="n">
+        <v>234.4</v>
+      </c>
+      <c r="N599" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="O599" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="P599" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q599" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="R599" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="S599" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="T599" t="n">
+        <v>2403</v>
+      </c>
+      <c r="U599" t="n">
+        <v>1</v>
+      </c>
+      <c r="V599" t="n">
+        <v>48.6</v>
+      </c>
+      <c r="W599" t="n">
+        <v>37638.6</v>
+      </c>
+      <c r="X599" t="n">
+        <v>3727</v>
+      </c>
+      <c r="Y599" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z599" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AA599" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AB599" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AC599" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AD599" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AE599" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AF599" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG599" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AH599" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI599" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ599" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK599" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL599" t="inlineStr"/>
+      <c r="AM599" t="inlineStr"/>
+    </row>
+    <row r="600">
+      <c r="A600" s="1" t="n">
+        <v>45335.71732638889</v>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C600" t="n">
+        <v>547.7</v>
+      </c>
+      <c r="D600" t="n">
+        <v>455.3</v>
+      </c>
+      <c r="E600" t="n">
+        <v>533.5</v>
+      </c>
+      <c r="F600" t="n">
+        <v>483.4</v>
+      </c>
+      <c r="G600" t="n">
+        <v>1</v>
+      </c>
+      <c r="H600" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="I600" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J600" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K600" t="n">
+        <v>232.6</v>
+      </c>
+      <c r="L600" t="n">
+        <v>232.4</v>
+      </c>
+      <c r="M600" t="n">
+        <v>234.2</v>
+      </c>
+      <c r="N600" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="O600" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="P600" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="Q600" t="n">
+        <v>59.97</v>
+      </c>
+      <c r="R600" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="S600" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="T600" t="n">
+        <v>2178</v>
+      </c>
+      <c r="U600" t="n">
+        <v>1</v>
+      </c>
+      <c r="V600" t="n">
+        <v>49.1</v>
+      </c>
+      <c r="W600" t="n">
+        <v>37638.8</v>
+      </c>
+      <c r="X600" t="n">
+        <v>3728</v>
+      </c>
+      <c r="Y600" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z600" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AA600" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AB600" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AC600" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AD600" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AE600" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AF600" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG600" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AH600" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI600" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ600" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK600" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL600" t="inlineStr"/>
+      <c r="AM600" t="inlineStr"/>
+    </row>
+    <row r="601">
+      <c r="A601" s="1" t="n">
+        <v>45335.72079861111</v>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C601" t="n">
+        <v>540.5</v>
+      </c>
+      <c r="D601" t="n">
+        <v>439.9</v>
+      </c>
+      <c r="E601" t="n">
+        <v>568.4</v>
+      </c>
+      <c r="F601" t="n">
+        <v>462.4</v>
+      </c>
+      <c r="G601" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H601" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I601" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J601" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K601" t="n">
+        <v>232.8</v>
+      </c>
+      <c r="L601" t="n">
+        <v>232.4</v>
+      </c>
+      <c r="M601" t="n">
+        <v>234</v>
+      </c>
+      <c r="N601" t="n">
+        <v>5</v>
+      </c>
+      <c r="O601" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="P601" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="Q601" t="n">
+        <v>59.97</v>
+      </c>
+      <c r="R601" t="n">
+        <v>59.95</v>
+      </c>
+      <c r="S601" t="n">
+        <v>59.96</v>
+      </c>
+      <c r="T601" t="n">
+        <v>1922</v>
+      </c>
+      <c r="U601" t="n">
+        <v>1</v>
+      </c>
+      <c r="V601" t="n">
+        <v>49.4</v>
+      </c>
+      <c r="W601" t="n">
+        <v>37638.9</v>
+      </c>
+      <c r="X601" t="n">
+        <v>3728</v>
+      </c>
+      <c r="Y601" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z601" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA601" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AB601" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AC601" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AD601" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AE601" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AF601" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG601" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AH601" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI601" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ601" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK601" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL601" t="inlineStr"/>
+      <c r="AM601" t="inlineStr"/>
+    </row>
+    <row r="602">
+      <c r="A602" s="1" t="n">
+        <v>45335.72427083334</v>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C602" t="n">
+        <v>547.3</v>
+      </c>
+      <c r="D602" t="n">
+        <v>452</v>
+      </c>
+      <c r="E602" t="n">
+        <v>560.5</v>
+      </c>
+      <c r="F602" t="n">
+        <v>542.3</v>
+      </c>
+      <c r="G602" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H602" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="I602" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J602" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="K602" t="n">
+        <v>232.6</v>
+      </c>
+      <c r="L602" t="n">
+        <v>232.2</v>
+      </c>
+      <c r="M602" t="n">
+        <v>234.2</v>
+      </c>
+      <c r="N602" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="O602" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="P602" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="Q602" t="n">
+        <v>59.96</v>
+      </c>
+      <c r="R602" t="n">
+        <v>59.97</v>
+      </c>
+      <c r="S602" t="n">
+        <v>59.96</v>
+      </c>
+      <c r="T602" t="n">
+        <v>1667</v>
+      </c>
+      <c r="U602" t="n">
+        <v>1</v>
+      </c>
+      <c r="V602" t="n">
+        <v>49.7</v>
+      </c>
+      <c r="W602" t="n">
+        <v>37639.1</v>
+      </c>
+      <c r="X602" t="n">
+        <v>3728</v>
+      </c>
+      <c r="Y602" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z602" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA602" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AB602" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AC602" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AD602" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AE602" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AF602" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG602" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AH602" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI602" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ602" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK602" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL602" t="inlineStr"/>
+      <c r="AM602" t="inlineStr"/>
+    </row>
+    <row r="603">
+      <c r="A603" s="1" t="n">
+        <v>45335.72774305556</v>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C603" t="n">
+        <v>538.5</v>
+      </c>
+      <c r="D603" t="n">
+        <v>439.1</v>
+      </c>
+      <c r="E603" t="n">
+        <v>539.1</v>
+      </c>
+      <c r="F603" t="n">
+        <v>558.8</v>
+      </c>
+      <c r="G603" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H603" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="I603" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J603" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K603" t="n">
+        <v>232.6</v>
+      </c>
+      <c r="L603" t="n">
+        <v>232.2</v>
+      </c>
+      <c r="M603" t="n">
+        <v>234.2</v>
+      </c>
+      <c r="N603" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="O603" t="n">
+        <v>4</v>
+      </c>
+      <c r="P603" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q603" t="n">
+        <v>59.95</v>
+      </c>
+      <c r="R603" t="n">
+        <v>59.96</v>
+      </c>
+      <c r="S603" t="n">
+        <v>59.93</v>
+      </c>
+      <c r="T603" t="n">
+        <v>1606</v>
+      </c>
+      <c r="U603" t="n">
+        <v>1</v>
+      </c>
+      <c r="V603" t="n">
+        <v>49.9</v>
+      </c>
+      <c r="W603" t="n">
+        <v>37639.2</v>
+      </c>
+      <c r="X603" t="n">
+        <v>3728</v>
+      </c>
+      <c r="Y603" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z603" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AA603" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AB603" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AC603" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AD603" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AE603" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AF603" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG603" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AH603" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI603" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ603" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK603" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL603" t="inlineStr"/>
+      <c r="AM603" t="inlineStr"/>
+    </row>
+    <row r="604">
+      <c r="A604" s="1" t="n">
+        <v>45335.73121527778</v>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C604" t="n">
+        <v>513.2</v>
+      </c>
+      <c r="D604" t="n">
+        <v>437.7</v>
+      </c>
+      <c r="E604" t="n">
+        <v>562.2</v>
+      </c>
+      <c r="F604" t="n">
+        <v>552</v>
+      </c>
+      <c r="G604" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H604" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="I604" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J604" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K604" t="n">
+        <v>232.6</v>
+      </c>
+      <c r="L604" t="n">
+        <v>232.2</v>
+      </c>
+      <c r="M604" t="n">
+        <v>234</v>
+      </c>
+      <c r="N604" t="n">
+        <v>4</v>
+      </c>
+      <c r="O604" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="P604" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q604" t="n">
+        <v>59.96</v>
+      </c>
+      <c r="R604" t="n">
+        <v>59.97</v>
+      </c>
+      <c r="S604" t="n">
+        <v>59.97</v>
+      </c>
+      <c r="T604" t="n">
+        <v>1559</v>
+      </c>
+      <c r="U604" t="n">
+        <v>1</v>
+      </c>
+      <c r="V604" t="n">
+        <v>50.1</v>
+      </c>
+      <c r="W604" t="n">
+        <v>37639.4</v>
+      </c>
+      <c r="X604" t="n">
+        <v>3728</v>
+      </c>
+      <c r="Y604" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z604" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AA604" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AB604" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AC604" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AD604" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AE604" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AF604" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG604" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AH604" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI604" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ604" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK604" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL604" t="inlineStr"/>
+      <c r="AM604" t="inlineStr"/>
+    </row>
+    <row r="605">
+      <c r="A605" s="1" t="n">
+        <v>45335.7346875</v>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C605" t="n">
+        <v>549.5</v>
+      </c>
+      <c r="D605" t="n">
+        <v>443.9</v>
+      </c>
+      <c r="E605" t="n">
+        <v>534.1</v>
+      </c>
+      <c r="F605" t="n">
+        <v>556</v>
+      </c>
+      <c r="G605" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H605" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="I605" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J605" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K605" t="n">
+        <v>232.4</v>
+      </c>
+      <c r="L605" t="n">
+        <v>232.4</v>
+      </c>
+      <c r="M605" t="n">
+        <v>234.4</v>
+      </c>
+      <c r="N605" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="O605" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="P605" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="Q605" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="R605" t="n">
+        <v>60.01</v>
+      </c>
+      <c r="S605" t="n">
+        <v>60.01</v>
+      </c>
+      <c r="T605" t="n">
+        <v>1450</v>
+      </c>
+      <c r="U605" t="n">
+        <v>1</v>
+      </c>
+      <c r="V605" t="n">
+        <v>48.8</v>
+      </c>
+      <c r="W605" t="n">
+        <v>37639.5</v>
+      </c>
+      <c r="X605" t="n">
+        <v>3728</v>
+      </c>
+      <c r="Y605" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z605" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AA605" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AB605" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AC605" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AD605" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AE605" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AF605" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG605" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AH605" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI605" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ605" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK605" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL605" t="inlineStr"/>
+      <c r="AM605" t="inlineStr"/>
+    </row>
+    <row r="606">
+      <c r="A606" s="1" t="n">
+        <v>45335.7381712963</v>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C606" t="n">
+        <v>511.1</v>
+      </c>
+      <c r="D606" t="n">
+        <v>436.9</v>
+      </c>
+      <c r="E606" t="n">
+        <v>557.2</v>
+      </c>
+      <c r="F606" t="n">
+        <v>543.2</v>
+      </c>
+      <c r="G606" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H606" t="n">
+        <v>1</v>
+      </c>
+      <c r="I606" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J606" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K606" t="n">
+        <v>232.4</v>
+      </c>
+      <c r="L606" t="n">
+        <v>232.2</v>
+      </c>
+      <c r="M606" t="n">
+        <v>234</v>
+      </c>
+      <c r="N606" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="O606" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="P606" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="Q606" t="n">
+        <v>59.97</v>
+      </c>
+      <c r="R606" t="n">
+        <v>59.96</v>
+      </c>
+      <c r="S606" t="n">
+        <v>59.95</v>
+      </c>
+      <c r="T606" t="n">
+        <v>1233</v>
+      </c>
+      <c r="U606" t="n">
+        <v>1</v>
+      </c>
+      <c r="V606" t="n">
+        <v>47.8</v>
+      </c>
+      <c r="W606" t="n">
+        <v>37639.6</v>
+      </c>
+      <c r="X606" t="n">
+        <v>3728</v>
+      </c>
+      <c r="Y606" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z606" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AA606" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AB606" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AC606" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AD606" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AE606" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AF606" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG606" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AH606" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI606" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ606" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK606" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL606" t="inlineStr"/>
+      <c r="AM606" t="inlineStr"/>
+    </row>
+    <row r="607">
+      <c r="A607" s="1" t="n">
+        <v>45335.74164351852</v>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C607" t="n">
+        <v>542.3</v>
+      </c>
+      <c r="D607" t="n">
+        <v>438.1</v>
+      </c>
+      <c r="E607" t="n">
+        <v>532.7</v>
+      </c>
+      <c r="F607" t="n">
+        <v>541.7</v>
+      </c>
+      <c r="G607" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H607" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="I607" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J607" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K607" t="n">
+        <v>232.6</v>
+      </c>
+      <c r="L607" t="n">
+        <v>232.2</v>
+      </c>
+      <c r="M607" t="n">
+        <v>234</v>
+      </c>
+      <c r="N607" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="O607" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="P607" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="Q607" t="n">
+        <v>59.93</v>
+      </c>
+      <c r="R607" t="n">
+        <v>59.93</v>
+      </c>
+      <c r="S607" t="n">
+        <v>59.93</v>
+      </c>
+      <c r="T607" t="n">
+        <v>992</v>
+      </c>
+      <c r="U607" t="n">
+        <v>1</v>
+      </c>
+      <c r="V607" t="n">
+        <v>47.4</v>
+      </c>
+      <c r="W607" t="n">
+        <v>37639.7</v>
+      </c>
+      <c r="X607" t="n">
+        <v>3728</v>
+      </c>
+      <c r="Y607" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z607" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AA607" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB607" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AC607" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AD607" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AE607" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF607" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG607" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AH607" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI607" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ607" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK607" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL607" t="inlineStr"/>
+      <c r="AM607" t="inlineStr"/>
+    </row>
+    <row r="608">
+      <c r="A608" s="1" t="n">
+        <v>45335.74510416666</v>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C608" t="n">
+        <v>541.4</v>
+      </c>
+      <c r="D608" t="n">
+        <v>422</v>
+      </c>
+      <c r="E608" t="n">
+        <v>524.8</v>
+      </c>
+      <c r="F608" t="n">
+        <v>509.3</v>
+      </c>
+      <c r="G608" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H608" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I608" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J608" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K608" t="n">
+        <v>233.2</v>
+      </c>
+      <c r="L608" t="n">
+        <v>232.4</v>
+      </c>
+      <c r="M608" t="n">
+        <v>234.4</v>
+      </c>
+      <c r="N608" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="O608" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="P608" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q608" t="n">
+        <v>59.94</v>
+      </c>
+      <c r="R608" t="n">
+        <v>59.94</v>
+      </c>
+      <c r="S608" t="n">
+        <v>59.95</v>
+      </c>
+      <c r="T608" t="n">
+        <v>710</v>
+      </c>
+      <c r="U608" t="n">
+        <v>1</v>
+      </c>
+      <c r="V608" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="W608" t="n">
+        <v>37639.8</v>
+      </c>
+      <c r="X608" t="n">
+        <v>3728</v>
+      </c>
+      <c r="Y608" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z608" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AA608" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB608" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AC608" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AD608" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE608" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AF608" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG608" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AH608" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI608" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ608" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK608" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL608" t="inlineStr"/>
+      <c r="AM608" t="inlineStr"/>
+    </row>
+    <row r="609">
+      <c r="A609" s="1" t="n">
+        <v>45335.74857638889</v>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C609" t="n">
+        <v>519.5</v>
+      </c>
+      <c r="D609" t="n">
+        <v>415.9</v>
+      </c>
+      <c r="E609" t="n">
+        <v>515.3</v>
+      </c>
+      <c r="F609" t="n">
+        <v>510.2</v>
+      </c>
+      <c r="G609" t="n">
+        <v>0</v>
+      </c>
+      <c r="H609" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="I609" t="n">
+        <v>0</v>
+      </c>
+      <c r="J609" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K609" t="n">
+        <v>232.8</v>
+      </c>
+      <c r="L609" t="n">
+        <v>232.8</v>
+      </c>
+      <c r="M609" t="n">
+        <v>234.6</v>
+      </c>
+      <c r="N609" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="O609" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="P609" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="Q609" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="R609" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="S609" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="T609" t="n">
+        <v>455</v>
+      </c>
+      <c r="U609" t="n">
+        <v>1</v>
+      </c>
+      <c r="V609" t="n">
+        <v>48</v>
+      </c>
+      <c r="W609" t="n">
+        <v>37639.8</v>
+      </c>
+      <c r="X609" t="n">
+        <v>3728</v>
+      </c>
+      <c r="Y609" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z609" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AA609" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB609" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC609" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AD609" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE609" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF609" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG609" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AH609" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI609" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ609" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK609" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL609" t="inlineStr"/>
+      <c r="AM609" t="inlineStr"/>
+    </row>
+    <row r="610">
+      <c r="A610" s="1" t="n">
+        <v>45335.75204861111</v>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C610" t="n">
+        <v>500.6</v>
+      </c>
+      <c r="D610" t="n">
+        <v>395.8</v>
+      </c>
+      <c r="E610" t="n">
+        <v>564.6</v>
+      </c>
+      <c r="F610" t="n">
+        <v>484.8</v>
+      </c>
+      <c r="G610" t="n">
+        <v>0</v>
+      </c>
+      <c r="H610" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I610" t="n">
+        <v>0</v>
+      </c>
+      <c r="J610" t="n">
+        <v>0</v>
+      </c>
+      <c r="K610" t="n">
+        <v>233</v>
+      </c>
+      <c r="L610" t="n">
+        <v>232</v>
+      </c>
+      <c r="M610" t="n">
+        <v>234.6</v>
+      </c>
+      <c r="N610" t="n">
+        <v>1</v>
+      </c>
+      <c r="O610" t="n">
+        <v>1</v>
+      </c>
+      <c r="P610" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Q610" t="n">
+        <v>59.95</v>
+      </c>
+      <c r="R610" t="n">
+        <v>59.94</v>
+      </c>
+      <c r="S610" t="n">
+        <v>59.96</v>
+      </c>
+      <c r="T610" t="n">
+        <v>152</v>
+      </c>
+      <c r="U610" t="n">
+        <v>1</v>
+      </c>
+      <c r="V610" t="n">
+        <v>49.1</v>
+      </c>
+      <c r="W610" t="n">
+        <v>37639.8</v>
+      </c>
+      <c r="X610" t="n">
+        <v>3728</v>
+      </c>
+      <c r="Y610" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z610" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA610" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB610" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC610" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD610" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE610" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF610" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG610" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AH610" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI610" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ610" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK610" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL610" t="inlineStr"/>
+      <c r="AM610" t="inlineStr"/>
+    </row>
+    <row r="611">
+      <c r="A611" s="1" t="n">
+        <v>45335.75552083334</v>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C611" t="n">
+        <v>570.2</v>
+      </c>
+      <c r="D611" t="n">
+        <v>418.9</v>
+      </c>
+      <c r="E611" t="n">
+        <v>495.8</v>
+      </c>
+      <c r="F611" t="n">
+        <v>525.2</v>
+      </c>
+      <c r="G611" t="n">
+        <v>0</v>
+      </c>
+      <c r="H611" t="n">
+        <v>0</v>
+      </c>
+      <c r="I611" t="n">
+        <v>0</v>
+      </c>
+      <c r="J611" t="n">
+        <v>0</v>
+      </c>
+      <c r="K611" t="n">
+        <v>232.6</v>
+      </c>
+      <c r="L611" t="n">
+        <v>232.2</v>
+      </c>
+      <c r="M611" t="n">
+        <v>234</v>
+      </c>
+      <c r="N611" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O611" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="P611" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Q611" t="n">
+        <v>59.89</v>
+      </c>
+      <c r="R611" t="n">
+        <v>59.94</v>
+      </c>
+      <c r="S611" t="n">
+        <v>59.91</v>
+      </c>
+      <c r="T611" t="n">
+        <v>5</v>
+      </c>
+      <c r="U611" t="n">
+        <v>1</v>
+      </c>
+      <c r="V611" t="n">
+        <v>50</v>
+      </c>
+      <c r="W611" t="n">
+        <v>37639.8</v>
+      </c>
+      <c r="X611" t="n">
+        <v>3728</v>
+      </c>
+      <c r="Y611" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z611" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA611" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB611" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC611" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD611" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE611" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF611" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG611" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH611" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI611" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ611" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK611" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL611" t="inlineStr"/>
+      <c r="AM611" t="inlineStr"/>
+    </row>
+    <row r="612">
+      <c r="A612" s="1" t="n">
+        <v>45335.75900462963</v>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C612" t="n">
+        <v>211.3</v>
+      </c>
+      <c r="D612" t="n">
+        <v>199.5</v>
+      </c>
+      <c r="E612" t="n">
+        <v>191.4</v>
+      </c>
+      <c r="F612" t="n">
+        <v>386.5</v>
+      </c>
+      <c r="G612" t="n">
+        <v>0</v>
+      </c>
+      <c r="H612" t="n">
+        <v>0</v>
+      </c>
+      <c r="I612" t="n">
+        <v>0</v>
+      </c>
+      <c r="J612" t="n">
+        <v>0</v>
+      </c>
+      <c r="K612" t="n">
+        <v>232</v>
+      </c>
+      <c r="L612" t="n">
+        <v>232</v>
+      </c>
+      <c r="M612" t="n">
+        <v>233.6</v>
+      </c>
+      <c r="N612" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O612" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P612" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="Q612" t="n">
+        <v>59.94</v>
+      </c>
+      <c r="R612" t="n">
+        <v>59.93</v>
+      </c>
+      <c r="S612" t="n">
+        <v>59.93</v>
+      </c>
+      <c r="T612" t="n">
+        <v>30</v>
+      </c>
+      <c r="U612" t="n">
+        <v>1</v>
+      </c>
+      <c r="V612" t="n">
+        <v>49.8</v>
+      </c>
+      <c r="W612" t="n">
+        <v>37639.8</v>
+      </c>
+      <c r="X612" t="n">
+        <v>3729</v>
+      </c>
+      <c r="Y612" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z612" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA612" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB612" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC612" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD612" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE612" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF612" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG612" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AH612" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI612" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ612" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK612" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL612" t="inlineStr"/>
+      <c r="AM612" t="inlineStr"/>
+    </row>
+    <row r="613">
+      <c r="A613" s="1" t="n">
+        <v>45335.76247685185</v>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C613" t="n">
+        <v>182.1</v>
+      </c>
+      <c r="D613" t="n">
+        <v>168.2</v>
+      </c>
+      <c r="E613" t="n">
+        <v>179.2</v>
+      </c>
+      <c r="F613" t="n">
+        <v>437.2</v>
+      </c>
+      <c r="G613" t="n">
+        <v>0</v>
+      </c>
+      <c r="H613" t="n">
+        <v>0</v>
+      </c>
+      <c r="I613" t="n">
+        <v>0</v>
+      </c>
+      <c r="J613" t="n">
+        <v>0</v>
+      </c>
+      <c r="K613" t="n">
+        <v>231.8</v>
+      </c>
+      <c r="L613" t="n">
+        <v>232.2</v>
+      </c>
+      <c r="M613" t="n">
+        <v>233</v>
+      </c>
+      <c r="N613" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O613" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="P613" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="Q613" t="n">
+        <v>59.85</v>
+      </c>
+      <c r="R613" t="n">
+        <v>59.87</v>
+      </c>
+      <c r="S613" t="n">
+        <v>59.86</v>
+      </c>
+      <c r="T613" t="n">
+        <v>4</v>
+      </c>
+      <c r="U613" t="n">
+        <v>1</v>
+      </c>
+      <c r="V613" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="W613" t="n">
+        <v>37639.8</v>
+      </c>
+      <c r="X613" t="n">
+        <v>3729</v>
+      </c>
+      <c r="Y613" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z613" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA613" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB613" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC613" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD613" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE613" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF613" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AG613" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH613" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI613" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ613" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK613" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL613" t="inlineStr"/>
+      <c r="AM613" t="inlineStr"/>
+    </row>
+    <row r="614">
+      <c r="A614" s="1" t="n">
+        <v>45335.76594907408</v>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C614" t="n">
+        <v>200</v>
+      </c>
+      <c r="D614" t="n">
+        <v>196.1</v>
+      </c>
+      <c r="E614" t="n">
+        <v>208.3</v>
+      </c>
+      <c r="F614" t="n">
+        <v>197.9</v>
+      </c>
+      <c r="G614" t="n">
+        <v>0</v>
+      </c>
+      <c r="H614" t="n">
+        <v>0</v>
+      </c>
+      <c r="I614" t="n">
+        <v>0</v>
+      </c>
+      <c r="J614" t="n">
+        <v>0</v>
+      </c>
+      <c r="K614" t="n">
+        <v>231.8</v>
+      </c>
+      <c r="L614" t="n">
+        <v>231.8</v>
+      </c>
+      <c r="M614" t="n">
+        <v>233.2</v>
+      </c>
+      <c r="N614" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O614" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="P614" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="Q614" t="n">
+        <v>59.92</v>
+      </c>
+      <c r="R614" t="n">
+        <v>59.92</v>
+      </c>
+      <c r="S614" t="n">
+        <v>59.92</v>
+      </c>
+      <c r="T614" t="n">
+        <v>7</v>
+      </c>
+      <c r="U614" t="n">
+        <v>1</v>
+      </c>
+      <c r="V614" t="n">
+        <v>49</v>
+      </c>
+      <c r="W614" t="n">
+        <v>37639.8</v>
+      </c>
+      <c r="X614" t="n">
+        <v>3729</v>
+      </c>
+      <c r="Y614" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z614" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA614" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB614" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC614" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD614" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE614" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF614" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG614" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AH614" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI614" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ614" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK614" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL614" t="inlineStr"/>
+      <c r="AM614" t="inlineStr"/>
+    </row>
+    <row r="615">
+      <c r="A615" s="1" t="n">
+        <v>45335.7694212963</v>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C615" t="n">
+        <v>201.8</v>
+      </c>
+      <c r="D615" t="n">
+        <v>202.8</v>
+      </c>
+      <c r="E615" t="n">
+        <v>200.7</v>
+      </c>
+      <c r="F615" t="n">
+        <v>200.8</v>
+      </c>
+      <c r="G615" t="n">
+        <v>0</v>
+      </c>
+      <c r="H615" t="n">
+        <v>0</v>
+      </c>
+      <c r="I615" t="n">
+        <v>0</v>
+      </c>
+      <c r="J615" t="n">
+        <v>0</v>
+      </c>
+      <c r="K615" t="n">
+        <v>231.2</v>
+      </c>
+      <c r="L615" t="n">
+        <v>231.6</v>
+      </c>
+      <c r="M615" t="n">
+        <v>232.4</v>
+      </c>
+      <c r="N615" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="O615" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="P615" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="Q615" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="R615" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="S615" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="T615" t="n">
+        <v>5</v>
+      </c>
+      <c r="U615" t="n">
+        <v>1</v>
+      </c>
+      <c r="V615" t="n">
+        <v>48.4</v>
+      </c>
+      <c r="W615" t="n">
+        <v>37639.8</v>
+      </c>
+      <c r="X615" t="n">
+        <v>3729</v>
+      </c>
+      <c r="Y615" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z615" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA615" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB615" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC615" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD615" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE615" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF615" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG615" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH615" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI615" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ615" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK615" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL615" t="inlineStr"/>
+      <c r="AM615" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>